<commit_message>
included Email messaging to confirm when a pipeline has completed usccessfully or unsuccessfully. Added validation_functions.py
</commit_message>
<xml_diff>
--- a/nfl_stats.xlsx
+++ b/nfl_stats.xlsx
@@ -130,12 +130,12 @@
     <t>32</t>
   </si>
   <si>
+    <t>Washington</t>
+  </si>
+  <si>
     <t>Baltimore</t>
   </si>
   <si>
-    <t>Washington</t>
-  </si>
-  <si>
     <t>Detroit</t>
   </si>
   <si>
@@ -304,12 +304,12 @@
     <t>11.7</t>
   </si>
   <si>
+    <t>32.3</t>
+  </si>
+  <si>
     <t>37.3</t>
   </si>
   <si>
-    <t>32.3</t>
-  </si>
-  <si>
     <t>40.0</t>
   </si>
   <si>
@@ -457,12 +457,12 @@
     <t>7.8</t>
   </si>
   <si>
+    <t>30.8</t>
+  </si>
+  <si>
     <t>32.5</t>
   </si>
   <si>
-    <t>30.8</t>
-  </si>
-  <si>
     <t>32.7</t>
   </si>
   <si>
@@ -1390,12 +1390,12 @@
     <t>38.46%</t>
   </si>
   <si>
+    <t>23.26%</t>
+  </si>
+  <si>
     <t>24.24%</t>
   </si>
   <si>
-    <t>23.26%</t>
-  </si>
-  <si>
     <t>39.13%</t>
   </si>
   <si>
@@ -1576,12 +1576,12 @@
     <t>+2.0</t>
   </si>
   <si>
+    <t>-1.3</t>
+  </si>
+  <si>
     <t>-0.7</t>
   </si>
   <si>
-    <t>-1.3</t>
-  </si>
-  <si>
     <t>-2.0</t>
   </si>
   <si>
@@ -2125,19 +2125,19 @@
     <t>62.79%</t>
   </si>
   <si>
+    <t>47.92%</t>
+  </si>
+  <si>
     <t>63.27%</t>
   </si>
   <si>
-    <t>47.92%</t>
+    <t>53.42%</t>
   </si>
   <si>
     <t>49.12%</t>
   </si>
   <si>
     <t>48.89%</t>
-  </si>
-  <si>
-    <t>53.42%</t>
   </si>
   <si>
     <t>50.85%</t>
@@ -2574,16 +2574,16 @@
         <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
         <v>144</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2600,16 +2600,16 @@
         <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
         <v>145</v>
       </c>
       <c r="H3" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2649,7 +2649,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
         <v>116</v>
@@ -4086,7 +4086,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>227</v>
@@ -4112,7 +4112,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>227</v>
@@ -4671,7 +4671,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>151</v>
@@ -4957,7 +4957,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>73</v>
@@ -5204,22 +5204,22 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>219</v>
       </c>
       <c r="D3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" t="s">
         <v>219</v>
       </c>
-      <c r="E3" t="s">
-        <v>239</v>
-      </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="G3" t="s">
-        <v>236</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
         <v>244</v>
@@ -5230,22 +5230,22 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>219</v>
       </c>
       <c r="D4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" t="s">
         <v>223</v>
       </c>
-      <c r="E4" t="s">
-        <v>219</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>236</v>
-      </c>
-      <c r="G4" t="s">
-        <v>132</v>
       </c>
       <c r="H4" t="s">
         <v>244</v>
@@ -5334,7 +5334,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>221</v>
@@ -5464,7 +5464,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>223</v>
@@ -5476,13 +5476,13 @@
         <v>228</v>
       </c>
       <c r="F13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>225</v>
       </c>
       <c r="H13" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5490,25 +5490,25 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="E14" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" t="s">
+        <v>244</v>
+      </c>
+      <c r="G14" t="s">
         <v>132</v>
       </c>
-      <c r="F14" t="s">
-        <v>219</v>
-      </c>
-      <c r="G14" t="s">
-        <v>229</v>
-      </c>
       <c r="H14" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -5516,25 +5516,25 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>223</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E15" t="s">
-        <v>228</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="G15" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="H15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -5750,25 +5750,25 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>228</v>
       </c>
       <c r="D24" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E24" t="s">
+        <v>228</v>
+      </c>
+      <c r="F24" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H24" t="s">
         <v>132</v>
-      </c>
-      <c r="F24" t="s">
-        <v>244</v>
-      </c>
-      <c r="G24" t="s">
-        <v>237</v>
-      </c>
-      <c r="H24" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -5776,7 +5776,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>228</v>
@@ -5785,16 +5785,16 @@
         <v>230</v>
       </c>
       <c r="E25" t="s">
-        <v>241</v>
+        <v>132</v>
       </c>
       <c r="F25" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="G25" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="H25" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -5802,25 +5802,25 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
         <v>228</v>
       </c>
       <c r="D26" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="F26" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="G26" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="H26" t="s">
-        <v>132</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -6075,7 +6075,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>254</v>
@@ -6101,7 +6101,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>255</v>
@@ -6972,7 +6972,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>237</v>
@@ -7180,7 +7180,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>225</v>
@@ -8025,25 +8025,25 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
         <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>306</v>
+        <v>336</v>
       </c>
       <c r="E11" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="F11" t="s">
-        <v>298</v>
+        <v>417</v>
       </c>
       <c r="G11" t="s">
         <v>455</v>
       </c>
       <c r="H11" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -8051,25 +8051,25 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
         <v>400</v>
       </c>
       <c r="D12" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
       <c r="E12" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="F12" t="s">
-        <v>417</v>
+        <v>298</v>
       </c>
       <c r="G12" t="s">
         <v>456</v>
       </c>
       <c r="H12" t="s">
-        <v>454</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -8363,7 +8363,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>410</v>
@@ -8493,7 +8493,7 @@
         <v>217</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>414</v>
@@ -8714,25 +8714,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>498</v>
       </c>
       <c r="D4" t="s">
-        <v>498</v>
+        <v>515</v>
       </c>
       <c r="E4" t="s">
-        <v>511</v>
+        <v>241</v>
       </c>
       <c r="F4" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
       <c r="G4" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
       <c r="H4" t="s">
-        <v>241</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -8740,25 +8740,25 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
         <v>498</v>
       </c>
       <c r="D5" t="s">
+        <v>516</v>
+      </c>
+      <c r="E5" t="s">
+        <v>498</v>
+      </c>
+      <c r="F5" t="s">
         <v>515</v>
       </c>
-      <c r="E5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" t="s">
-        <v>502</v>
-      </c>
       <c r="G5" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="H5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -8766,25 +8766,25 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>498</v>
       </c>
       <c r="D6" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="E6" t="s">
-        <v>498</v>
+        <v>511</v>
       </c>
       <c r="F6" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="G6" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="H6" t="s">
-        <v>503</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -8836,7 +8836,7 @@
         <v>500</v>
       </c>
       <c r="H8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -8856,7 +8856,7 @@
         <v>521</v>
       </c>
       <c r="F9" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G9" t="s">
         <v>497</v>
@@ -8870,7 +8870,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>501</v>
@@ -8896,22 +8896,22 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>502</v>
       </c>
       <c r="D11" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F11" t="s">
+        <v>241</v>
+      </c>
+      <c r="G11" t="s">
         <v>500</v>
-      </c>
-      <c r="E11" t="s">
-        <v>516</v>
-      </c>
-      <c r="F11" t="s">
-        <v>517</v>
-      </c>
-      <c r="G11" t="s">
-        <v>498</v>
       </c>
       <c r="H11" t="s">
         <v>530</v>
@@ -8922,7 +8922,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>502</v>
@@ -8931,16 +8931,16 @@
         <v>500</v>
       </c>
       <c r="E12" t="s">
+        <v>516</v>
+      </c>
+      <c r="F12" t="s">
+        <v>518</v>
+      </c>
+      <c r="G12" t="s">
         <v>498</v>
       </c>
-      <c r="F12" t="s">
-        <v>524</v>
-      </c>
-      <c r="G12" t="s">
-        <v>506</v>
-      </c>
       <c r="H12" t="s">
-        <v>504</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -8948,25 +8948,25 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>502</v>
       </c>
       <c r="D13" t="s">
+        <v>500</v>
+      </c>
+      <c r="E13" t="s">
+        <v>498</v>
+      </c>
+      <c r="F13" t="s">
+        <v>524</v>
+      </c>
+      <c r="G13" t="s">
         <v>506</v>
       </c>
-      <c r="E13" t="s">
-        <v>511</v>
-      </c>
-      <c r="F13" t="s">
-        <v>525</v>
-      </c>
-      <c r="G13" t="s">
-        <v>241</v>
-      </c>
       <c r="H13" t="s">
-        <v>530</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -8974,22 +8974,22 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>502</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>506</v>
       </c>
       <c r="E14" t="s">
         <v>511</v>
       </c>
       <c r="F14" t="s">
+        <v>525</v>
+      </c>
+      <c r="G14" t="s">
         <v>241</v>
-      </c>
-      <c r="G14" t="s">
-        <v>500</v>
       </c>
       <c r="H14" t="s">
         <v>530</v>
@@ -9015,7 +9015,7 @@
         <v>498</v>
       </c>
       <c r="G15" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="H15" t="s">
         <v>531</v>
@@ -9078,7 +9078,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>504</v>
@@ -9182,25 +9182,25 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>507</v>
       </c>
       <c r="D22" t="s">
+        <v>517</v>
+      </c>
+      <c r="E22" t="s">
+        <v>519</v>
+      </c>
+      <c r="F22" t="s">
         <v>241</v>
       </c>
-      <c r="E22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F22" t="s">
-        <v>511</v>
-      </c>
       <c r="G22" t="s">
-        <v>502</v>
+        <v>529</v>
       </c>
       <c r="H22" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -9208,25 +9208,25 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
         <v>507</v>
       </c>
       <c r="D23" t="s">
+        <v>506</v>
+      </c>
+      <c r="E23" t="s">
+        <v>519</v>
+      </c>
+      <c r="F23" t="s">
         <v>517</v>
       </c>
-      <c r="E23" t="s">
-        <v>520</v>
-      </c>
-      <c r="F23" t="s">
-        <v>511</v>
-      </c>
       <c r="G23" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="H23" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -9234,25 +9234,25 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>507</v>
       </c>
       <c r="D24" t="s">
-        <v>518</v>
+        <v>241</v>
       </c>
       <c r="E24" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="F24" t="s">
-        <v>241</v>
+        <v>511</v>
       </c>
       <c r="G24" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="H24" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -9260,25 +9260,25 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>507</v>
       </c>
       <c r="D25" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="E25" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F25" t="s">
+        <v>511</v>
+      </c>
+      <c r="G25" t="s">
+        <v>498</v>
+      </c>
+      <c r="H25" t="s">
         <v>518</v>
-      </c>
-      <c r="G25" t="s">
-        <v>502</v>
-      </c>
-      <c r="H25" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -9286,25 +9286,25 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
         <v>508</v>
       </c>
       <c r="D26" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="E26" t="s">
-        <v>498</v>
+        <v>511</v>
       </c>
       <c r="F26" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G26" t="s">
         <v>506</v>
       </c>
       <c r="H26" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -9312,25 +9312,25 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>508</v>
       </c>
       <c r="D27" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="E27" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="F27" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G27" t="s">
         <v>506</v>
       </c>
       <c r="H27" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -9344,7 +9344,7 @@
         <v>509</v>
       </c>
       <c r="D28" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E28" t="s">
         <v>241</v>
@@ -9396,7 +9396,7 @@
         <v>511</v>
       </c>
       <c r="D30" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E30" t="s">
         <v>241</v>
@@ -9405,7 +9405,7 @@
         <v>508</v>
       </c>
       <c r="G30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H30" t="s">
         <v>509</v>
@@ -9448,7 +9448,7 @@
         <v>512</v>
       </c>
       <c r="D32" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E32" t="s">
         <v>519</v>
@@ -9457,7 +9457,7 @@
         <v>527</v>
       </c>
       <c r="G32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H32" t="s">
         <v>507</v>
@@ -9480,7 +9480,7 @@
         <v>520</v>
       </c>
       <c r="F33" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G33" t="s">
         <v>526</v>
@@ -9845,7 +9845,7 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>196</v>
@@ -10287,7 +10287,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
         <v>559</v>
@@ -10404,7 +10404,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>657</v>
@@ -10742,22 +10742,22 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>670</v>
       </c>
       <c r="D15" t="s">
-        <v>316</v>
+        <v>666</v>
       </c>
       <c r="E15" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" t="s">
+        <v>666</v>
+      </c>
+      <c r="G15" t="s">
         <v>254</v>
-      </c>
-      <c r="F15" t="s">
-        <v>278</v>
-      </c>
-      <c r="G15" t="s">
-        <v>690</v>
       </c>
       <c r="H15" t="s">
         <v>700</v>
@@ -10768,25 +10768,25 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
         <v>670</v>
       </c>
       <c r="D16" t="s">
-        <v>666</v>
+        <v>254</v>
       </c>
       <c r="E16" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
       <c r="F16" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="G16" t="s">
         <v>254</v>
       </c>
       <c r="H16" t="s">
-        <v>701</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -10794,25 +10794,25 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>670</v>
       </c>
       <c r="D17" t="s">
+        <v>316</v>
+      </c>
+      <c r="E17" t="s">
         <v>254</v>
       </c>
-      <c r="E17" t="s">
-        <v>681</v>
-      </c>
       <c r="F17" t="s">
-        <v>664</v>
+        <v>278</v>
       </c>
       <c r="G17" t="s">
-        <v>254</v>
+        <v>690</v>
       </c>
       <c r="H17" t="s">
-        <v>254</v>
+        <v>701</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -10846,22 +10846,22 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>672</v>
       </c>
       <c r="D19" t="s">
-        <v>318</v>
+        <v>664</v>
       </c>
       <c r="E19" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
       <c r="F19" t="s">
-        <v>309</v>
+        <v>665</v>
       </c>
       <c r="G19" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="H19" t="s">
         <v>702</v>
@@ -10872,19 +10872,19 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
         <v>672</v>
       </c>
       <c r="D20" t="s">
-        <v>664</v>
+        <v>318</v>
       </c>
       <c r="E20" t="s">
-        <v>664</v>
+        <v>278</v>
       </c>
       <c r="F20" t="s">
-        <v>668</v>
+        <v>309</v>
       </c>
       <c r="G20" t="s">
         <v>254</v>
@@ -10898,7 +10898,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
         <v>672</v>
@@ -10907,13 +10907,13 @@
         <v>664</v>
       </c>
       <c r="E21" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
       <c r="F21" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="G21" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="H21" t="s">
         <v>704</v>
@@ -10976,25 +10976,25 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>254</v>
       </c>
       <c r="D24" t="s">
-        <v>309</v>
+        <v>668</v>
       </c>
       <c r="E24" t="s">
-        <v>681</v>
+        <v>321</v>
       </c>
       <c r="F24" t="s">
-        <v>447</v>
+        <v>272</v>
       </c>
       <c r="G24" t="s">
-        <v>318</v>
+        <v>684</v>
       </c>
       <c r="H24" t="s">
-        <v>707</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -11002,25 +11002,25 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>254</v>
       </c>
       <c r="D25" t="s">
-        <v>668</v>
+        <v>309</v>
       </c>
       <c r="E25" t="s">
-        <v>321</v>
+        <v>681</v>
       </c>
       <c r="F25" t="s">
-        <v>272</v>
+        <v>447</v>
       </c>
       <c r="G25" t="s">
-        <v>684</v>
+        <v>318</v>
       </c>
       <c r="H25" t="s">
-        <v>254</v>
+        <v>707</v>
       </c>
     </row>
     <row r="26" spans="1:8">

</xml_diff>